<commit_message>
add new post, update readme
</commit_message>
<xml_diff>
--- a/people_temp.xlsx
+++ b/people_temp.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Name</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>Dr. Todd Gibson</t>
+  </si>
+  <si>
+    <t>Dr. Edward Roualdes</t>
   </si>
 </sst>
 </file>
@@ -437,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F85E9C6-E0BF-4C9B-B4D1-D0BD184F3DA3}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,6 +505,11 @@
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>